<commit_message>
client & group Scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3530-RBI-EI-DB-SAR-REC-NON-RNI-CTPD-SAR-MD-TR-1-INSTALLMENT-FEE-FLAT-PREPAY-PERIODIC-Newcreateloan.xlsx
+++ b/Mifos Automation Excels/Client/3530-RBI-EI-DB-SAR-REC-NON-RNI-CTPD-SAR-MD-TR-1-INSTALLMENT-FEE-FLAT-PREPAY-PERIODIC-Newcreateloan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>waittopageload</t>
-  </si>
-  <si>
-    <t>waittopageload2</t>
   </si>
 </sst>
 </file>
@@ -786,10 +783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,17 +837,9 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="15">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B6" s="15" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1140,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>